<commit_message>
First full working version
</commit_message>
<xml_diff>
--- a/Inputs_Data_largePlans/NMR_Comparison_raw.xlsx
+++ b/Inputs_Data_largePlans/NMR_Comparison_raw.xlsx
@@ -1541,7 +1541,7 @@
         <v>0.0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.05908295562044133</v>
+        <v>0.05331039138987579</v>
       </c>
       <c r="G3" t="n">
         <v>0.0</v>
@@ -1550,7 +1550,7 @@
         <v>0.0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.05776102704901276</v>
+        <v>0.05198846281844722</v>
       </c>
       <c r="J3" t="n">
         <v>0.0</v>
@@ -1576,19 +1576,19 @@
         <v>0.0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.03342525047639681</v>
+        <v>0.03054070656352176</v>
       </c>
       <c r="G4" t="n">
-        <v>0.07168097844581409</v>
+        <v>0.1453078904717736</v>
       </c>
       <c r="H4" t="n">
         <v>0.0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.03223617904782538</v>
+        <v>0.029351635134950333</v>
       </c>
       <c r="J4" t="n">
-        <v>0.07049190701724266</v>
+        <v>0.14411881904320215</v>
       </c>
       <c r="K4" t="n">
         <v>0.0</v>
@@ -1611,19 +1611,19 @@
         <v>0.0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.027249271209058085</v>
+        <v>0.025129467108006374</v>
       </c>
       <c r="G5" t="n">
-        <v>0.032879018628217654</v>
+        <v>0.04659224249893037</v>
       </c>
       <c r="H5" t="n">
         <v>0.0</v>
       </c>
       <c r="I5" t="n">
-        <v>0.026545128351915227</v>
+        <v>0.024425324250863516</v>
       </c>
       <c r="J5" t="n">
-        <v>0.03182280434250337</v>
+        <v>0.04553602821321608</v>
       </c>
       <c r="K5" t="n">
         <v>0.0</v>
@@ -1646,22 +1646,22 @@
         <v>0.04663985714285714</v>
       </c>
       <c r="F6" t="n">
-        <v>0.07772593116931138</v>
+        <v>0.07657326248711238</v>
       </c>
       <c r="G6" t="n">
-        <v>0.06928553270324059</v>
+        <v>0.07040603735437492</v>
       </c>
       <c r="H6" t="n">
-        <v>0.09274520992296315</v>
+        <v>0.18770442345298777</v>
       </c>
       <c r="I6" t="n">
-        <v>0.022077382227050104</v>
+        <v>0.020924713544851106</v>
       </c>
       <c r="J6" t="n">
-        <v>0.022645675560383438</v>
+        <v>0.023766180211517773</v>
       </c>
       <c r="K6" t="n">
-        <v>0.046105352780106</v>
+        <v>0.14106456631013062</v>
       </c>
     </row>
     <row r="7">
@@ -1681,22 +1681,22 @@
         <v>0.048720294539991826</v>
       </c>
       <c r="F7" t="n">
-        <v>0.10332651597309686</v>
+        <v>0.108168586394391</v>
       </c>
       <c r="G7" t="n">
-        <v>0.061612630190475304</v>
+        <v>0.06751898285526695</v>
       </c>
       <c r="H7" t="n">
-        <v>0.06528369335397097</v>
+        <v>0.08954536183624093</v>
       </c>
       <c r="I7" t="n">
-        <v>0.012679479201783984</v>
+        <v>0.017521549623078135</v>
       </c>
       <c r="J7" t="n">
-        <v>0.012892335650483481</v>
+        <v>0.01879868831527512</v>
       </c>
       <c r="K7" t="n">
-        <v>0.016563398813979145</v>
+        <v>0.0408250672962491</v>
       </c>
     </row>
     <row r="8">
@@ -1716,22 +1716,22 @@
         <v>0.07882907633849179</v>
       </c>
       <c r="F8" t="n">
-        <v>0.150967163560386</v>
+        <v>0.15541945590358547</v>
       </c>
       <c r="G8" t="n">
-        <v>0.10202334120438364</v>
+        <v>0.1071633510318814</v>
       </c>
       <c r="H8" t="n">
-        <v>0.09191644125283455</v>
+        <v>0.09942663073889114</v>
       </c>
       <c r="I8" t="n">
-        <v>0.012577715390533241</v>
+        <v>0.017030007733732686</v>
       </c>
       <c r="J8" t="n">
-        <v>0.012692334971249627</v>
+        <v>0.01783234479874739</v>
       </c>
       <c r="K8" t="n">
-        <v>0.013087364914342764</v>
+        <v>0.020597554400399353</v>
       </c>
     </row>
     <row r="9">
@@ -1751,22 +1751,22 @@
         <v>0.10849313705099367</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2268151839296687</v>
+        <v>0.2287182902740183</v>
       </c>
       <c r="G9" t="n">
-        <v>0.17989187641212898</v>
+        <v>0.18196677340452938</v>
       </c>
       <c r="H9" t="n">
-        <v>0.12486401137310138</v>
+        <v>0.12805640472117413</v>
       </c>
       <c r="I9" t="n">
-        <v>0.016186690464432964</v>
+        <v>0.01808979680878255</v>
       </c>
       <c r="J9" t="n">
-        <v>0.01621123198558308</v>
+        <v>0.018286128977983478</v>
       </c>
       <c r="K9" t="n">
-        <v>0.016370874322107702</v>
+        <v>0.01956326767018046</v>
       </c>
     </row>
     <row r="10">
@@ -1786,22 +1786,22 @@
         <v>0.19596484615011464</v>
       </c>
       <c r="F10" t="n">
-        <v>0.288169597612782</v>
+        <v>0.29040071964001773</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2799438817363919</v>
+        <v>0.2818455149101809</v>
       </c>
       <c r="H10" t="n">
-        <v>0.21201018365581023</v>
+        <v>0.2146250053318345</v>
       </c>
       <c r="I10" t="n">
-        <v>0.015997375049597015</v>
+        <v>0.01822849707683276</v>
       </c>
       <c r="J10" t="n">
-        <v>0.015956188942916172</v>
+        <v>0.01785782211670517</v>
       </c>
       <c r="K10" t="n">
-        <v>0.016045337505695582</v>
+        <v>0.01866015918171987</v>
       </c>
     </row>
     <row r="11">
@@ -1821,22 +1821,22 @@
         <v>0.38685835897295157</v>
       </c>
       <c r="F11" t="n">
-        <v>0.40973876582866564</v>
+        <v>0.4194297881336389</v>
       </c>
       <c r="G11" t="n">
-        <v>0.4125978763973669</v>
+        <v>0.4217402668669335</v>
       </c>
       <c r="H11" t="n">
-        <v>0.3924634800198235</v>
+        <v>0.40178256944167096</v>
       </c>
       <c r="I11" t="n">
-        <v>0.005646446922774812</v>
+        <v>0.015337469227748111</v>
       </c>
       <c r="J11" t="n">
-        <v>0.005585487829951845</v>
+        <v>0.014727878299518448</v>
       </c>
       <c r="K11" t="n">
-        <v>0.005605121046871938</v>
+        <v>0.014924210468719374</v>
       </c>
     </row>
     <row r="12">
@@ -1856,22 +1856,22 @@
         <v>0.3805106914593575</v>
       </c>
       <c r="F12" t="n">
-        <v>0.37991739201412433</v>
+        <v>0.3898490913120772</v>
       </c>
       <c r="G12" t="n">
-        <v>0.38280338931491203</v>
+        <v>0.39239436500549935</v>
       </c>
       <c r="H12" t="n">
-        <v>0.3858094246381016</v>
+        <v>0.39506342309220926</v>
       </c>
       <c r="I12" t="n">
-        <v>0.005366503263128616</v>
+        <v>0.015298202561081446</v>
       </c>
       <c r="J12" t="n">
-        <v>0.005332430902392065</v>
+        <v>0.014923406592979372</v>
       </c>
       <c r="K12" t="n">
-        <v>0.005298733178744101</v>
+        <v>0.01455273163285178</v>
       </c>
     </row>
     <row r="13">
@@ -1926,7 +1926,7 @@
         <v>0.0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.04677927871417905</v>
+        <v>0.06408813614253714</v>
       </c>
       <c r="G14" t="n">
         <v>0.0</v>
@@ -1935,7 +1935,7 @@
         <v>0.0</v>
       </c>
       <c r="I14" t="n">
-        <v>0.04307787871417905</v>
+        <v>0.06038673614253714</v>
       </c>
       <c r="J14" t="n">
         <v>0.0</v>
@@ -1961,19 +1961,19 @@
         <v>0.0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.037836191228507426</v>
+        <v>0.04790435614253713</v>
       </c>
       <c r="G15" t="n">
-        <v>0.06552783016677355</v>
+        <v>0.18636255083386777</v>
       </c>
       <c r="H15" t="n">
         <v>0.0</v>
       </c>
       <c r="I15" t="n">
-        <v>0.03450679122850743</v>
+        <v>0.044574956142537134</v>
       </c>
       <c r="J15" t="n">
-        <v>0.06219843016677355</v>
+        <v>0.18303315083386776</v>
       </c>
       <c r="K15" t="n">
         <v>0.0</v>
@@ -1996,19 +1996,19 @@
         <v>0.0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.033239159448933873</v>
+        <v>0.043417616142537134</v>
       </c>
       <c r="G16" t="n">
-        <v>0.03623921659179102</v>
+        <v>0.05850321614253713</v>
       </c>
       <c r="H16" t="n">
         <v>0.0</v>
       </c>
       <c r="I16" t="n">
-        <v>0.031267559448933877</v>
+        <v>0.04144601614253714</v>
       </c>
       <c r="J16" t="n">
-        <v>0.03328181659179102</v>
+        <v>0.05554581614253713</v>
       </c>
       <c r="K16" t="n">
         <v>0.0</v>
@@ -2031,22 +2031,22 @@
         <v>0.0025916</v>
       </c>
       <c r="F17" t="n">
-        <v>0.027276417349170794</v>
+        <v>0.0369988228092038</v>
       </c>
       <c r="G17" t="n">
-        <v>0.029004150682504126</v>
+        <v>0.03872655614253714</v>
       </c>
       <c r="H17" t="n">
-        <v>0.044757616759318636</v>
+        <v>0.18050775083386777</v>
       </c>
       <c r="I17" t="n">
-        <v>0.026412550682504126</v>
+        <v>0.03613495614253714</v>
       </c>
       <c r="J17" t="n">
-        <v>0.026412550682504126</v>
+        <v>0.03613495614253714</v>
       </c>
       <c r="K17" t="n">
-        <v>0.042166016759318636</v>
+        <v>0.17791615083386778</v>
       </c>
     </row>
     <row r="18">
@@ -2066,22 +2066,22 @@
         <v>0.006018</v>
       </c>
       <c r="F18" t="n">
-        <v>0.017620368740230645</v>
+        <v>0.034664056142537134</v>
       </c>
       <c r="G18" t="n">
-        <v>0.017620368740230645</v>
+        <v>0.034664056142537134</v>
       </c>
       <c r="H18" t="n">
-        <v>0.018986777831139737</v>
+        <v>0.049694556142537136</v>
       </c>
       <c r="I18" t="n">
-        <v>0.011602368740230646</v>
+        <v>0.028646056142537134</v>
       </c>
       <c r="J18" t="n">
-        <v>0.011602368740230646</v>
+        <v>0.028646056142537134</v>
       </c>
       <c r="K18" t="n">
-        <v>0.012968777831139738</v>
+        <v>0.04367655614253713</v>
       </c>
     </row>
     <row r="19">
@@ -2101,22 +2101,22 @@
         <v>0.061368000000000006</v>
       </c>
       <c r="F19" t="n">
-        <v>0.07432192739557979</v>
+        <v>0.09256705614253714</v>
       </c>
       <c r="G19" t="n">
-        <v>0.07309526072891312</v>
+        <v>0.09134038947587048</v>
       </c>
       <c r="H19" t="n">
-        <v>0.07064192739557978</v>
+        <v>0.08888705614253714</v>
       </c>
       <c r="I19" t="n">
-        <v>0.009273927395579779</v>
+        <v>0.027519056142537135</v>
       </c>
       <c r="J19" t="n">
-        <v>0.009273927395579779</v>
+        <v>0.027519056142537135</v>
       </c>
       <c r="K19" t="n">
-        <v>0.009273927395579779</v>
+        <v>0.027519056142537135</v>
       </c>
     </row>
     <row r="20">
@@ -2136,22 +2136,22 @@
         <v>0.0981192467651161</v>
       </c>
       <c r="F20" t="n">
-        <v>0.16724937861640962</v>
+        <v>0.18717600434944429</v>
       </c>
       <c r="G20" t="n">
-        <v>0.11916703872740204</v>
+        <v>0.1390936644604367</v>
       </c>
       <c r="H20" t="n">
-        <v>0.10700157717461858</v>
+        <v>0.12692820290765325</v>
       </c>
       <c r="I20" t="n">
-        <v>0.008882330409502476</v>
+        <v>0.028808956142537135</v>
       </c>
       <c r="J20" t="n">
-        <v>0.008882330409502476</v>
+        <v>0.028808956142537135</v>
       </c>
       <c r="K20" t="n">
-        <v>0.008882330409502476</v>
+        <v>0.028808956142537135</v>
       </c>
     </row>
     <row r="21">
@@ -2171,22 +2171,22 @@
         <v>0.19759125342923495</v>
       </c>
       <c r="F21" t="n">
-        <v>0.24480514017593288</v>
+        <v>0.26581846360420314</v>
       </c>
       <c r="G21" t="n">
-        <v>0.2250267546930875</v>
+        <v>0.24604007812135775</v>
       </c>
       <c r="H21" t="n">
-        <v>0.20606908614350183</v>
+        <v>0.2270824095717721</v>
       </c>
       <c r="I21" t="n">
-        <v>0.00847783271426689</v>
+        <v>0.029491156142537136</v>
       </c>
       <c r="J21" t="n">
-        <v>0.00847783271426689</v>
+        <v>0.029491156142537136</v>
       </c>
       <c r="K21" t="n">
-        <v>0.00847783271426689</v>
+        <v>0.029491156142537136</v>
       </c>
     </row>
     <row r="22">
@@ -2206,22 +2206,22 @@
         <v>0.2300029651487684</v>
       </c>
       <c r="F22" t="n">
-        <v>0.23364868558129928</v>
+        <v>0.25346067561107133</v>
       </c>
       <c r="G22" t="n">
-        <v>0.24182488063356722</v>
+        <v>0.26163687066333924</v>
       </c>
       <c r="H22" t="n">
-        <v>0.2379581312615335</v>
+        <v>0.2577701212913055</v>
       </c>
       <c r="I22" t="n">
-        <v>0.007955166112765113</v>
+        <v>0.027767156142537136</v>
       </c>
       <c r="J22" t="n">
-        <v>0.007955166112765113</v>
+        <v>0.027767156142537136</v>
       </c>
       <c r="K22" t="n">
-        <v>0.007955166112765113</v>
+        <v>0.027767156142537136</v>
       </c>
     </row>
     <row r="23">
@@ -2241,22 +2241,22 @@
         <v>0.23351145641202536</v>
       </c>
       <c r="F23" t="n">
-        <v>0.22622868941493376</v>
+        <v>0.24631379050306437</v>
       </c>
       <c r="G23" t="n">
-        <v>0.23440488446720167</v>
+        <v>0.2544899855553323</v>
       </c>
       <c r="H23" t="n">
-        <v>0.2410757114664319</v>
+        <v>0.26116081255456247</v>
       </c>
       <c r="I23" t="n">
-        <v>0.00756425505440653</v>
+        <v>0.027649356142537135</v>
       </c>
       <c r="J23" t="n">
-        <v>0.00756425505440653</v>
+        <v>0.027649356142537135</v>
       </c>
       <c r="K23" t="n">
-        <v>0.00756425505440653</v>
+        <v>0.027649356142537135</v>
       </c>
     </row>
     <row r="24">
@@ -2696,7 +2696,7 @@
         <v>0.0</v>
       </c>
       <c r="F36" t="n">
-        <v>0.10166092194842105</v>
+        <v>0.08156797005810723</v>
       </c>
       <c r="G36" t="n">
         <v>0.0</v>
@@ -2705,7 +2705,7 @@
         <v>0.0</v>
       </c>
       <c r="I36" t="n">
-        <v>0.10166092194842105</v>
+        <v>0.08156797005810723</v>
       </c>
       <c r="J36" t="n">
         <v>0.0</v>
@@ -2731,19 +2731,19 @@
         <v>0.0</v>
       </c>
       <c r="F37" t="n">
-        <v>0.03619563179046619</v>
+        <v>0.03447518934582117</v>
       </c>
       <c r="G37" t="n">
-        <v>0.08791327077377203</v>
+        <v>0.1896281062957387</v>
       </c>
       <c r="H37" t="n">
         <v>0.0</v>
       </c>
       <c r="I37" t="n">
-        <v>0.03619563179046619</v>
+        <v>0.03447518934582117</v>
       </c>
       <c r="J37" t="n">
-        <v>0.08791327077377203</v>
+        <v>0.1896281062957387</v>
       </c>
       <c r="K37" t="n">
         <v>0.0</v>
@@ -2766,19 +2766,19 @@
         <v>0.0</v>
       </c>
       <c r="F38" t="n">
-        <v>0.023377761448086346</v>
+        <v>0.025672378321953206</v>
       </c>
       <c r="G38" t="n">
-        <v>0.03347983941985077</v>
+        <v>0.0660806902090109</v>
       </c>
       <c r="H38" t="n">
         <v>0.0</v>
       </c>
       <c r="I38" t="n">
-        <v>0.023377761448086346</v>
+        <v>0.025672378321953206</v>
       </c>
       <c r="J38" t="n">
-        <v>0.03347983941985077</v>
+        <v>0.0660806902090109</v>
       </c>
       <c r="K38" t="n">
         <v>0.0</v>
@@ -2801,22 +2801,22 @@
         <v>0.0</v>
       </c>
       <c r="F39" t="n">
-        <v>0.017692453156191945</v>
+        <v>0.02165367300976149</v>
       </c>
       <c r="G39" t="n">
-        <v>0.019069333156191946</v>
+        <v>0.028538073009761487</v>
       </c>
       <c r="H39" t="n">
-        <v>0.04781642817354446</v>
+        <v>0.17227354809652407</v>
       </c>
       <c r="I39" t="n">
-        <v>0.017692453156191945</v>
+        <v>0.02165367300976149</v>
       </c>
       <c r="J39" t="n">
-        <v>0.019069333156191946</v>
+        <v>0.028538073009761487</v>
       </c>
       <c r="K39" t="n">
-        <v>0.04781642817354446</v>
+        <v>0.17227354809652407</v>
       </c>
     </row>
     <row r="40">
@@ -2836,22 +2836,22 @@
         <v>0.0025000000000000005</v>
       </c>
       <c r="F40" t="n">
-        <v>0.018530657197462157</v>
+        <v>0.021997966421895603</v>
       </c>
       <c r="G40" t="n">
-        <v>0.019169226543560645</v>
+        <v>0.025829382498486556</v>
       </c>
       <c r="H40" t="n">
-        <v>0.025651866034047635</v>
+        <v>0.0647252194414085</v>
       </c>
       <c r="I40" t="n">
-        <v>0.016030657197462155</v>
+        <v>0.019497966421895604</v>
       </c>
       <c r="J40" t="n">
-        <v>0.016669226543560647</v>
+        <v>0.023329382498486553</v>
       </c>
       <c r="K40" t="n">
-        <v>0.023151866034047636</v>
+        <v>0.06222521944140849</v>
       </c>
     </row>
     <row r="41">
@@ -2871,22 +2871,22 @@
         <v>0.010374999999999999</v>
       </c>
       <c r="F41" t="n">
-        <v>0.16358977728037535</v>
+        <v>0.16262844096262752</v>
       </c>
       <c r="G41" t="n">
-        <v>0.030558636022524517</v>
+        <v>0.03166045215767163</v>
       </c>
       <c r="H41" t="n">
-        <v>0.03150944013751822</v>
+        <v>0.038316080962627515</v>
       </c>
       <c r="I41" t="n">
-        <v>0.01983977728037536</v>
+        <v>0.018878440962627516</v>
       </c>
       <c r="J41" t="n">
-        <v>0.02018363602252452</v>
+        <v>0.021285452157671633</v>
       </c>
       <c r="K41" t="n">
-        <v>0.021134440137518216</v>
+        <v>0.027941080962627516</v>
       </c>
     </row>
     <row r="42">
@@ -2906,22 +2906,22 @@
         <v>0.02436178012952881</v>
       </c>
       <c r="F42" t="n">
-        <v>0.2566826762428555</v>
+        <v>0.24647490865118427</v>
       </c>
       <c r="G42" t="n">
-        <v>0.06673445763229069</v>
+        <v>0.057042061984771894</v>
       </c>
       <c r="H42" t="n">
-        <v>0.056282533578034775</v>
+        <v>0.04994262699753305</v>
       </c>
       <c r="I42" t="n">
-        <v>0.03136820187548175</v>
+        <v>0.021160434283810516</v>
       </c>
       <c r="J42" t="n">
-        <v>0.0314418264389321</v>
+        <v>0.021749430791413293</v>
       </c>
       <c r="K42" t="n">
-        <v>0.031920753448505965</v>
+        <v>0.025580846868004242</v>
       </c>
     </row>
     <row r="43">
@@ -2941,22 +2941,22 @@
         <v>0.14145858143986056</v>
       </c>
       <c r="F43" t="n">
-        <v>0.32956878125506134</v>
+        <v>0.31896245298784665</v>
       </c>
       <c r="G43" t="n">
-        <v>0.32552235059459333</v>
+        <v>0.3139275557670384</v>
       </c>
       <c r="H43" t="n">
-        <v>0.17310313216333206</v>
+        <v>0.16364790284248304</v>
       </c>
       <c r="I43" t="n">
-        <v>0.03150066335517581</v>
+        <v>0.020894335087961142</v>
       </c>
       <c r="J43" t="n">
-        <v>0.031377105035133274</v>
+        <v>0.01978231020757837</v>
       </c>
       <c r="K43" t="n">
-        <v>0.03164455072347151</v>
+        <v>0.022189321402622482</v>
       </c>
     </row>
     <row r="44">
@@ -2976,22 +2976,22 @@
         <v>0.22092445215974643</v>
       </c>
       <c r="F44" t="n">
-        <v>0.2726569405792574</v>
+        <v>0.28520766696589384</v>
       </c>
       <c r="G44" t="n">
-        <v>0.27247406330078844</v>
+        <v>0.2833788941812049</v>
       </c>
       <c r="H44" t="n">
-        <v>0.22219499968610854</v>
+        <v>0.2336299274233674</v>
       </c>
       <c r="I44" t="n">
-        <v>0.0013945251540707201</v>
+        <v>0.0139452515407072</v>
       </c>
       <c r="J44" t="n">
-        <v>0.0012116478756018206</v>
+        <v>0.012116478756018206</v>
       </c>
       <c r="K44" t="n">
-        <v>0.0012705475263620986</v>
+        <v>0.012705475263620987</v>
       </c>
     </row>
     <row r="45">
@@ -3011,22 +3011,22 @@
         <v>0.2548617981829562</v>
       </c>
       <c r="F45" t="n">
-        <v>0.25382901640812683</v>
+        <v>0.2665065178087697</v>
       </c>
       <c r="G45" t="n">
-        <v>0.2537267993259172</v>
+        <v>0.2653821299044635</v>
       </c>
       <c r="H45" t="n">
-        <v>0.2559262380698669</v>
+        <v>0.26657063693897437</v>
       </c>
       <c r="I45" t="n">
-        <v>0.0012677501400642909</v>
+        <v>0.0139452515407072</v>
       </c>
       <c r="J45" t="n">
-        <v>0.0011655330578546346</v>
+        <v>0.01282086363640098</v>
       </c>
       <c r="K45" t="n">
-        <v>0.001064439886910746</v>
+        <v>0.011708838756018206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>